<commit_message>
Move RHPF to shift hydrogen to steam methane reforming; fix default hydrogen shifting FoPITY settings to 1 from 2025-2050; FoPITY edits for NDC scenario
</commit_message>
<xml_diff>
--- a/InputData/hydgn/RHPF/Recipient Hydrogen Pathway Fractions.xlsx
+++ b/InputData/hydgn/RHPF/Recipient Hydrogen Pathway Fractions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Modeling\EPS\US\eps-us\InputData\hydgn\RHPF\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganMahajan\Documents\eps-us\InputData\hydgn\RHPF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{626AD650-2600-4FD9-8DF7-DB8CE20BF1F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8AA43F9-77A7-447F-8C44-DDD7DF7C76CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31395" yWindow="1440" windowWidth="25290" windowHeight="13845" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -79,10 +79,10 @@
     <t>natural gas reforming with CCS</t>
   </si>
   <si>
-    <t>electrolysis that is guaranteed to be supplied by new clean electricity sources.</t>
-  </si>
-  <si>
     <t>hydrocarbon partial oxidation</t>
+  </si>
+  <si>
+    <t>steam methane reforming.</t>
   </si>
 </sst>
 </file>
@@ -427,14 +427,14 @@
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -442,42 +442,42 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>14</v>
       </c>
@@ -496,17 +496,17 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="B7" sqref="B7:H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.26953125" customWidth="1"/>
-    <col min="2" max="6" width="16.54296875" style="3" customWidth="1"/>
-    <col min="7" max="8" width="16.453125" customWidth="1"/>
+    <col min="1" max="1" width="34.28515625" customWidth="1"/>
+    <col min="2" max="6" width="16.5703125" style="3" customWidth="1"/>
+    <col min="7" max="8" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>13</v>
       </c>
@@ -523,7 +523,7 @@
         <v>12</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G1" s="5" t="s">
         <v>15</v>
@@ -532,7 +532,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -558,33 +558,33 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E3" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F3" s="3">
-        <v>0</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+      <c r="G3" s="3">
+        <v>1</v>
+      </c>
+      <c r="H3" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -610,7 +610,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -636,9 +636,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B6" s="3">
         <v>0</v>
@@ -662,33 +662,33 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>15</v>
       </c>
       <c r="B7" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C7" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D7" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E7" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F7" s="3">
-        <v>1</v>
-      </c>
-      <c r="G7">
-        <v>1</v>
-      </c>
-      <c r="H7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+      <c r="G7" s="3">
+        <v>0</v>
+      </c>
+      <c r="H7" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>16</v>
       </c>

</xml_diff>